<commit_message>
Most functions work now, working through setting new row position on successful swap
</commit_message>
<xml_diff>
--- a/Hanoi Grid Layout.xlsx
+++ b/Hanoi Grid Layout.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="24040" yWindow="0" windowWidth="14360" windowHeight="24000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="24000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="54">
   <si>
     <t>Footer</t>
   </si>
@@ -47,7 +47,148 @@
     <t>Base</t>
   </si>
   <si>
-    <t>Disc</t>
+    <t>Grid-Tower-1-1</t>
+  </si>
+  <si>
+    <t>Grid-Tower-1-2</t>
+  </si>
+  <si>
+    <t>Grid-Tower-1-14</t>
+  </si>
+  <si>
+    <t>Grid-Tower-1-13</t>
+  </si>
+  <si>
+    <t>Grid-Tower-1-12</t>
+  </si>
+  <si>
+    <t>Grid-Tower-1-11</t>
+  </si>
+  <si>
+    <t>Grid-Tower-1-10</t>
+  </si>
+  <si>
+    <t>Grid-Tower-1-9</t>
+  </si>
+  <si>
+    <t>Grid-Tower-1-8</t>
+  </si>
+  <si>
+    <t>Grid-Tower-1-7</t>
+  </si>
+  <si>
+    <t>Grid-Tower-1-6</t>
+  </si>
+  <si>
+    <t>Grid-Tower-1-5</t>
+  </si>
+  <si>
+    <t>Grid-Tower-1-4</t>
+  </si>
+  <si>
+    <t>Grid-Tower-1-3</t>
+  </si>
+  <si>
+    <t>Grid-Tower-2-1</t>
+  </si>
+  <si>
+    <t>Grid-Tower-2-2</t>
+  </si>
+  <si>
+    <t>Grid-Tower-2-16</t>
+  </si>
+  <si>
+    <t>Grid-Tower-2-15</t>
+  </si>
+  <si>
+    <t>Grid-Tower-2-14</t>
+  </si>
+  <si>
+    <t>Grid-Tower-2-13</t>
+  </si>
+  <si>
+    <t>Grid-Tower-2-12</t>
+  </si>
+  <si>
+    <t>Grid-Tower-2-11</t>
+  </si>
+  <si>
+    <t>Grid-Tower-2-10</t>
+  </si>
+  <si>
+    <t>Grid-Tower-2-9</t>
+  </si>
+  <si>
+    <t>Grid-Tower-2-8</t>
+  </si>
+  <si>
+    <t>Grid-Tower-2-7</t>
+  </si>
+  <si>
+    <t>Grid-Tower-2-6</t>
+  </si>
+  <si>
+    <t>Grid-Tower-2-5</t>
+  </si>
+  <si>
+    <t>Grid-Tower-2-4</t>
+  </si>
+  <si>
+    <t>Grid-Tower-2-3</t>
+  </si>
+  <si>
+    <t>Grid-Tower-1-16</t>
+  </si>
+  <si>
+    <t>Grid-Tower-1-15</t>
+  </si>
+  <si>
+    <t>Grid-Tower-3-1</t>
+  </si>
+  <si>
+    <t>Grid-Tower-3-2</t>
+  </si>
+  <si>
+    <t>Grid-Tower-3-15</t>
+  </si>
+  <si>
+    <t>Grid-Tower-3-14</t>
+  </si>
+  <si>
+    <t>Grid-Tower-3-13</t>
+  </si>
+  <si>
+    <t>Grid-Tower-3-12</t>
+  </si>
+  <si>
+    <t>Grid-Tower-3-11</t>
+  </si>
+  <si>
+    <t>Grid-Tower-3-10</t>
+  </si>
+  <si>
+    <t>Grid-Tower-3-9</t>
+  </si>
+  <si>
+    <t>Grid-Tower-3-8</t>
+  </si>
+  <si>
+    <t>Grid-Tower-3-7</t>
+  </si>
+  <si>
+    <t>Grid-Tower-3-6</t>
+  </si>
+  <si>
+    <t>Grid-Tower-3-5</t>
+  </si>
+  <si>
+    <t>Grid-Tower-3-4</t>
+  </si>
+  <si>
+    <t>Grid-Tower-3-3</t>
+  </si>
+  <si>
+    <t>Grid-Tower-3-16</t>
   </si>
 </sst>
 </file>
@@ -463,6 +604,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -490,103 +649,85 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -868,9 +1009,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE30"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="Z10" sqref="Z10:AD25"/>
-    </sheetView>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -884,26 +1023,26 @@
       <c r="D1" s="2"/>
       <c r="E1" s="7"/>
       <c r="F1" s="9"/>
-      <c r="G1" s="43" t="s">
+      <c r="G1" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
-      <c r="N1" s="44"/>
-      <c r="O1" s="44"/>
-      <c r="P1" s="44"/>
-      <c r="Q1" s="44"/>
-      <c r="R1" s="44"/>
-      <c r="S1" s="44"/>
-      <c r="T1" s="44"/>
-      <c r="U1" s="44"/>
-      <c r="V1" s="44"/>
-      <c r="W1" s="44"/>
-      <c r="X1" s="45"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="43"/>
+      <c r="P1" s="43"/>
+      <c r="Q1" s="43"/>
+      <c r="R1" s="43"/>
+      <c r="S1" s="43"/>
+      <c r="T1" s="43"/>
+      <c r="U1" s="43"/>
+      <c r="V1" s="43"/>
+      <c r="W1" s="43"/>
+      <c r="X1" s="44"/>
       <c r="Y1" s="9"/>
       <c r="Z1" s="2"/>
       <c r="AA1" s="2"/>
@@ -918,24 +1057,24 @@
       <c r="D2" s="5"/>
       <c r="E2" s="8"/>
       <c r="F2" s="10"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="47"/>
-      <c r="K2" s="47"/>
-      <c r="L2" s="47"/>
-      <c r="M2" s="47"/>
-      <c r="N2" s="47"/>
-      <c r="O2" s="47"/>
-      <c r="P2" s="47"/>
-      <c r="Q2" s="47"/>
-      <c r="R2" s="47"/>
-      <c r="S2" s="47"/>
-      <c r="T2" s="47"/>
-      <c r="U2" s="47"/>
-      <c r="V2" s="47"/>
-      <c r="W2" s="47"/>
-      <c r="X2" s="48"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="46"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="46"/>
+      <c r="N2" s="46"/>
+      <c r="O2" s="46"/>
+      <c r="P2" s="46"/>
+      <c r="Q2" s="46"/>
+      <c r="R2" s="46"/>
+      <c r="S2" s="46"/>
+      <c r="T2" s="46"/>
+      <c r="U2" s="46"/>
+      <c r="V2" s="46"/>
+      <c r="W2" s="46"/>
+      <c r="X2" s="47"/>
       <c r="Y2" s="10"/>
       <c r="Z2" s="5"/>
       <c r="AA2" s="5"/>
@@ -950,24 +1089,24 @@
       <c r="D3" s="5"/>
       <c r="E3" s="8"/>
       <c r="F3" s="10"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="47"/>
-      <c r="K3" s="47"/>
-      <c r="L3" s="47"/>
-      <c r="M3" s="47"/>
-      <c r="N3" s="47"/>
-      <c r="O3" s="47"/>
-      <c r="P3" s="47"/>
-      <c r="Q3" s="47"/>
-      <c r="R3" s="47"/>
-      <c r="S3" s="47"/>
-      <c r="T3" s="47"/>
-      <c r="U3" s="47"/>
-      <c r="V3" s="47"/>
-      <c r="W3" s="47"/>
-      <c r="X3" s="48"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="46"/>
+      <c r="L3" s="46"/>
+      <c r="M3" s="46"/>
+      <c r="N3" s="46"/>
+      <c r="O3" s="46"/>
+      <c r="P3" s="46"/>
+      <c r="Q3" s="46"/>
+      <c r="R3" s="46"/>
+      <c r="S3" s="46"/>
+      <c r="T3" s="46"/>
+      <c r="U3" s="46"/>
+      <c r="V3" s="46"/>
+      <c r="W3" s="46"/>
+      <c r="X3" s="47"/>
       <c r="Y3" s="10"/>
       <c r="Z3" s="5"/>
       <c r="AA3" s="5"/>
@@ -982,24 +1121,24 @@
       <c r="D4" s="5"/>
       <c r="E4" s="8"/>
       <c r="F4" s="10"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="47"/>
-      <c r="K4" s="47"/>
-      <c r="L4" s="47"/>
-      <c r="M4" s="47"/>
-      <c r="N4" s="47"/>
-      <c r="O4" s="47"/>
-      <c r="P4" s="47"/>
-      <c r="Q4" s="47"/>
-      <c r="R4" s="47"/>
-      <c r="S4" s="47"/>
-      <c r="T4" s="47"/>
-      <c r="U4" s="47"/>
-      <c r="V4" s="47"/>
-      <c r="W4" s="47"/>
-      <c r="X4" s="48"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="46"/>
+      <c r="K4" s="46"/>
+      <c r="L4" s="46"/>
+      <c r="M4" s="46"/>
+      <c r="N4" s="46"/>
+      <c r="O4" s="46"/>
+      <c r="P4" s="46"/>
+      <c r="Q4" s="46"/>
+      <c r="R4" s="46"/>
+      <c r="S4" s="46"/>
+      <c r="T4" s="46"/>
+      <c r="U4" s="46"/>
+      <c r="V4" s="46"/>
+      <c r="W4" s="46"/>
+      <c r="X4" s="47"/>
       <c r="Y4" s="10"/>
       <c r="Z4" s="5"/>
       <c r="AA4" s="5"/>
@@ -1014,24 +1153,24 @@
       <c r="D5" s="12"/>
       <c r="E5" s="13"/>
       <c r="F5" s="14"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="50"/>
-      <c r="I5" s="50"/>
-      <c r="J5" s="50"/>
-      <c r="K5" s="50"/>
-      <c r="L5" s="50"/>
-      <c r="M5" s="50"/>
-      <c r="N5" s="50"/>
-      <c r="O5" s="50"/>
-      <c r="P5" s="50"/>
-      <c r="Q5" s="50"/>
-      <c r="R5" s="50"/>
-      <c r="S5" s="50"/>
-      <c r="T5" s="50"/>
-      <c r="U5" s="50"/>
-      <c r="V5" s="50"/>
-      <c r="W5" s="50"/>
-      <c r="X5" s="51"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="49"/>
+      <c r="J5" s="49"/>
+      <c r="K5" s="49"/>
+      <c r="L5" s="49"/>
+      <c r="M5" s="49"/>
+      <c r="N5" s="49"/>
+      <c r="O5" s="49"/>
+      <c r="P5" s="49"/>
+      <c r="Q5" s="49"/>
+      <c r="R5" s="49"/>
+      <c r="S5" s="49"/>
+      <c r="T5" s="49"/>
+      <c r="U5" s="49"/>
+      <c r="V5" s="49"/>
+      <c r="W5" s="49"/>
+      <c r="X5" s="50"/>
       <c r="Y5" s="14"/>
       <c r="Z5" s="12"/>
       <c r="AA5" s="12"/>
@@ -1084,26 +1223,26 @@
       <c r="D7" s="5"/>
       <c r="E7" s="8"/>
       <c r="F7" s="10"/>
-      <c r="G7" s="52" t="s">
+      <c r="G7" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="53"/>
-      <c r="I7" s="53"/>
-      <c r="J7" s="53"/>
-      <c r="K7" s="53"/>
-      <c r="L7" s="53"/>
-      <c r="M7" s="53"/>
-      <c r="N7" s="53"/>
-      <c r="O7" s="53"/>
-      <c r="P7" s="53"/>
-      <c r="Q7" s="53"/>
-      <c r="R7" s="53"/>
-      <c r="S7" s="53"/>
-      <c r="T7" s="53"/>
-      <c r="U7" s="53"/>
-      <c r="V7" s="53"/>
-      <c r="W7" s="53"/>
-      <c r="X7" s="54"/>
+      <c r="H7" s="52"/>
+      <c r="I7" s="52"/>
+      <c r="J7" s="52"/>
+      <c r="K7" s="52"/>
+      <c r="L7" s="52"/>
+      <c r="M7" s="52"/>
+      <c r="N7" s="52"/>
+      <c r="O7" s="52"/>
+      <c r="P7" s="52"/>
+      <c r="Q7" s="52"/>
+      <c r="R7" s="52"/>
+      <c r="S7" s="52"/>
+      <c r="T7" s="52"/>
+      <c r="U7" s="52"/>
+      <c r="V7" s="52"/>
+      <c r="W7" s="52"/>
+      <c r="X7" s="53"/>
       <c r="Y7" s="10"/>
       <c r="Z7" s="5"/>
       <c r="AA7" s="5"/>
@@ -1118,24 +1257,24 @@
       <c r="D8" s="12"/>
       <c r="E8" s="13"/>
       <c r="F8" s="14"/>
-      <c r="G8" s="55"/>
-      <c r="H8" s="56"/>
-      <c r="I8" s="56"/>
-      <c r="J8" s="56"/>
-      <c r="K8" s="56"/>
-      <c r="L8" s="56"/>
-      <c r="M8" s="56"/>
-      <c r="N8" s="56"/>
-      <c r="O8" s="56"/>
-      <c r="P8" s="56"/>
-      <c r="Q8" s="56"/>
-      <c r="R8" s="56"/>
-      <c r="S8" s="56"/>
-      <c r="T8" s="56"/>
-      <c r="U8" s="56"/>
-      <c r="V8" s="56"/>
-      <c r="W8" s="56"/>
-      <c r="X8" s="57"/>
+      <c r="G8" s="54"/>
+      <c r="H8" s="55"/>
+      <c r="I8" s="55"/>
+      <c r="J8" s="55"/>
+      <c r="K8" s="55"/>
+      <c r="L8" s="55"/>
+      <c r="M8" s="55"/>
+      <c r="N8" s="55"/>
+      <c r="O8" s="55"/>
+      <c r="P8" s="55"/>
+      <c r="Q8" s="55"/>
+      <c r="R8" s="55"/>
+      <c r="S8" s="55"/>
+      <c r="T8" s="55"/>
+      <c r="U8" s="55"/>
+      <c r="V8" s="55"/>
+      <c r="W8" s="55"/>
+      <c r="X8" s="56"/>
       <c r="Y8" s="14"/>
       <c r="Z8" s="12"/>
       <c r="AA8" s="12"/>
@@ -1182,16 +1321,16 @@
       </c>
     </row>
     <row r="10" spans="1:31" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="23"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="29"/>
       <c r="F10" s="10"/>
       <c r="G10" s="60" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="H10" s="61"/>
       <c r="I10" s="61"/>
@@ -1199,7 +1338,7 @@
       <c r="K10" s="61"/>
       <c r="L10" s="62"/>
       <c r="M10" s="60" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="N10" s="61"/>
       <c r="O10" s="61"/>
@@ -1207,7 +1346,7 @@
       <c r="Q10" s="61"/>
       <c r="R10" s="62"/>
       <c r="S10" s="60" t="s">
-        <v>6</v>
+        <v>53</v>
       </c>
       <c r="T10" s="61"/>
       <c r="U10" s="61"/>
@@ -1215,26 +1354,26 @@
       <c r="W10" s="61"/>
       <c r="X10" s="62"/>
       <c r="Y10" s="10"/>
-      <c r="Z10" s="37" t="s">
+      <c r="Z10" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="AA10" s="22"/>
-      <c r="AB10" s="22"/>
-      <c r="AC10" s="22"/>
-      <c r="AD10" s="38"/>
+      <c r="AA10" s="28"/>
+      <c r="AB10" s="28"/>
+      <c r="AC10" s="28"/>
+      <c r="AD10" s="37"/>
       <c r="AE10">
         <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:31" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="24"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="26"/>
+      <c r="A11" s="30"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="32"/>
       <c r="F11" s="10"/>
       <c r="G11" s="60" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="H11" s="61"/>
       <c r="I11" s="61"/>
@@ -1242,7 +1381,7 @@
       <c r="K11" s="61"/>
       <c r="L11" s="62"/>
       <c r="M11" s="60" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="N11" s="61"/>
       <c r="O11" s="61"/>
@@ -1250,7 +1389,7 @@
       <c r="Q11" s="61"/>
       <c r="R11" s="62"/>
       <c r="S11" s="60" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="T11" s="61"/>
       <c r="U11" s="61"/>
@@ -1258,24 +1397,24 @@
       <c r="W11" s="61"/>
       <c r="X11" s="62"/>
       <c r="Y11" s="10"/>
-      <c r="Z11" s="39"/>
-      <c r="AA11" s="25"/>
-      <c r="AB11" s="25"/>
-      <c r="AC11" s="25"/>
-      <c r="AD11" s="40"/>
+      <c r="Z11" s="38"/>
+      <c r="AA11" s="31"/>
+      <c r="AB11" s="31"/>
+      <c r="AC11" s="31"/>
+      <c r="AD11" s="39"/>
       <c r="AE11">
         <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:31" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="24"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="26"/>
+      <c r="A12" s="30"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="32"/>
       <c r="F12" s="10"/>
       <c r="G12" s="60" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H12" s="61"/>
       <c r="I12" s="61"/>
@@ -1283,7 +1422,7 @@
       <c r="K12" s="61"/>
       <c r="L12" s="62"/>
       <c r="M12" s="60" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="N12" s="61"/>
       <c r="O12" s="61"/>
@@ -1291,7 +1430,7 @@
       <c r="Q12" s="61"/>
       <c r="R12" s="62"/>
       <c r="S12" s="60" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="T12" s="61"/>
       <c r="U12" s="61"/>
@@ -1299,24 +1438,24 @@
       <c r="W12" s="61"/>
       <c r="X12" s="62"/>
       <c r="Y12" s="10"/>
-      <c r="Z12" s="39"/>
-      <c r="AA12" s="25"/>
-      <c r="AB12" s="25"/>
-      <c r="AC12" s="25"/>
-      <c r="AD12" s="40"/>
+      <c r="Z12" s="38"/>
+      <c r="AA12" s="31"/>
+      <c r="AB12" s="31"/>
+      <c r="AC12" s="31"/>
+      <c r="AD12" s="39"/>
       <c r="AE12">
         <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:31" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="24"/>
-      <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="26"/>
+      <c r="A13" s="30"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="32"/>
       <c r="F13" s="10"/>
       <c r="G13" s="60" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="H13" s="61"/>
       <c r="I13" s="61"/>
@@ -1324,7 +1463,7 @@
       <c r="K13" s="61"/>
       <c r="L13" s="62"/>
       <c r="M13" s="60" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="N13" s="61"/>
       <c r="O13" s="61"/>
@@ -1332,7 +1471,7 @@
       <c r="Q13" s="61"/>
       <c r="R13" s="62"/>
       <c r="S13" s="60" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="T13" s="61"/>
       <c r="U13" s="61"/>
@@ -1340,24 +1479,24 @@
       <c r="W13" s="61"/>
       <c r="X13" s="62"/>
       <c r="Y13" s="10"/>
-      <c r="Z13" s="39"/>
-      <c r="AA13" s="25"/>
-      <c r="AB13" s="25"/>
-      <c r="AC13" s="25"/>
-      <c r="AD13" s="40"/>
+      <c r="Z13" s="38"/>
+      <c r="AA13" s="31"/>
+      <c r="AB13" s="31"/>
+      <c r="AC13" s="31"/>
+      <c r="AD13" s="39"/>
       <c r="AE13">
         <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:31" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="24"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="26"/>
+      <c r="A14" s="30"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="32"/>
       <c r="F14" s="10"/>
       <c r="G14" s="60" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="H14" s="61"/>
       <c r="I14" s="61"/>
@@ -1365,7 +1504,7 @@
       <c r="K14" s="61"/>
       <c r="L14" s="62"/>
       <c r="M14" s="60" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="N14" s="61"/>
       <c r="O14" s="61"/>
@@ -1373,7 +1512,7 @@
       <c r="Q14" s="61"/>
       <c r="R14" s="62"/>
       <c r="S14" s="60" t="s">
-        <v>6</v>
+        <v>43</v>
       </c>
       <c r="T14" s="61"/>
       <c r="U14" s="61"/>
@@ -1381,24 +1520,24 @@
       <c r="W14" s="61"/>
       <c r="X14" s="62"/>
       <c r="Y14" s="10"/>
-      <c r="Z14" s="39"/>
-      <c r="AA14" s="25"/>
-      <c r="AB14" s="25"/>
-      <c r="AC14" s="25"/>
-      <c r="AD14" s="40"/>
+      <c r="Z14" s="38"/>
+      <c r="AA14" s="31"/>
+      <c r="AB14" s="31"/>
+      <c r="AC14" s="31"/>
+      <c r="AD14" s="39"/>
       <c r="AE14">
         <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:31" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="24"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="26"/>
+      <c r="A15" s="30"/>
+      <c r="B15" s="31"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="32"/>
       <c r="F15" s="10"/>
       <c r="G15" s="60" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="H15" s="61"/>
       <c r="I15" s="61"/>
@@ -1406,7 +1545,7 @@
       <c r="K15" s="61"/>
       <c r="L15" s="62"/>
       <c r="M15" s="60" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="N15" s="61"/>
       <c r="O15" s="61"/>
@@ -1414,7 +1553,7 @@
       <c r="Q15" s="61"/>
       <c r="R15" s="62"/>
       <c r="S15" s="60" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="T15" s="61"/>
       <c r="U15" s="61"/>
@@ -1422,24 +1561,24 @@
       <c r="W15" s="61"/>
       <c r="X15" s="62"/>
       <c r="Y15" s="10"/>
-      <c r="Z15" s="39"/>
-      <c r="AA15" s="25"/>
-      <c r="AB15" s="25"/>
-      <c r="AC15" s="25"/>
-      <c r="AD15" s="40"/>
+      <c r="Z15" s="38"/>
+      <c r="AA15" s="31"/>
+      <c r="AB15" s="31"/>
+      <c r="AC15" s="31"/>
+      <c r="AD15" s="39"/>
       <c r="AE15">
         <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:31" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="24"/>
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="26"/>
+      <c r="A16" s="30"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="32"/>
       <c r="F16" s="10"/>
       <c r="G16" s="60" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="H16" s="61"/>
       <c r="I16" s="61"/>
@@ -1447,7 +1586,7 @@
       <c r="K16" s="61"/>
       <c r="L16" s="62"/>
       <c r="M16" s="60" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="N16" s="61"/>
       <c r="O16" s="61"/>
@@ -1455,7 +1594,7 @@
       <c r="Q16" s="61"/>
       <c r="R16" s="62"/>
       <c r="S16" s="60" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="T16" s="61"/>
       <c r="U16" s="61"/>
@@ -1463,24 +1602,24 @@
       <c r="W16" s="61"/>
       <c r="X16" s="62"/>
       <c r="Y16" s="10"/>
-      <c r="Z16" s="39"/>
-      <c r="AA16" s="25"/>
-      <c r="AB16" s="25"/>
-      <c r="AC16" s="25"/>
-      <c r="AD16" s="40"/>
+      <c r="Z16" s="38"/>
+      <c r="AA16" s="31"/>
+      <c r="AB16" s="31"/>
+      <c r="AC16" s="31"/>
+      <c r="AD16" s="39"/>
       <c r="AE16">
         <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:31" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="24"/>
-      <c r="B17" s="25"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="26"/>
+      <c r="A17" s="30"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="32"/>
       <c r="F17" s="10"/>
       <c r="G17" s="60" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="H17" s="61"/>
       <c r="I17" s="61"/>
@@ -1488,7 +1627,7 @@
       <c r="K17" s="61"/>
       <c r="L17" s="62"/>
       <c r="M17" s="60" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="N17" s="61"/>
       <c r="O17" s="61"/>
@@ -1496,7 +1635,7 @@
       <c r="Q17" s="61"/>
       <c r="R17" s="62"/>
       <c r="S17" s="60" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="T17" s="61"/>
       <c r="U17" s="61"/>
@@ -1504,24 +1643,24 @@
       <c r="W17" s="61"/>
       <c r="X17" s="62"/>
       <c r="Y17" s="10"/>
-      <c r="Z17" s="39"/>
-      <c r="AA17" s="25"/>
-      <c r="AB17" s="25"/>
-      <c r="AC17" s="25"/>
-      <c r="AD17" s="40"/>
+      <c r="Z17" s="38"/>
+      <c r="AA17" s="31"/>
+      <c r="AB17" s="31"/>
+      <c r="AC17" s="31"/>
+      <c r="AD17" s="39"/>
       <c r="AE17">
         <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:31" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="24"/>
-      <c r="B18" s="25"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="26"/>
+      <c r="A18" s="30"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="32"/>
       <c r="F18" s="10"/>
       <c r="G18" s="60" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="H18" s="61"/>
       <c r="I18" s="61"/>
@@ -1529,7 +1668,7 @@
       <c r="K18" s="61"/>
       <c r="L18" s="62"/>
       <c r="M18" s="60" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="N18" s="61"/>
       <c r="O18" s="61"/>
@@ -1537,7 +1676,7 @@
       <c r="Q18" s="61"/>
       <c r="R18" s="62"/>
       <c r="S18" s="60" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="T18" s="61"/>
       <c r="U18" s="61"/>
@@ -1545,24 +1684,24 @@
       <c r="W18" s="61"/>
       <c r="X18" s="62"/>
       <c r="Y18" s="10"/>
-      <c r="Z18" s="39"/>
-      <c r="AA18" s="25"/>
-      <c r="AB18" s="25"/>
-      <c r="AC18" s="25"/>
-      <c r="AD18" s="40"/>
+      <c r="Z18" s="38"/>
+      <c r="AA18" s="31"/>
+      <c r="AB18" s="31"/>
+      <c r="AC18" s="31"/>
+      <c r="AD18" s="39"/>
       <c r="AE18">
         <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:31" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="24"/>
-      <c r="B19" s="25"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="26"/>
+      <c r="A19" s="30"/>
+      <c r="B19" s="31"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="32"/>
       <c r="F19" s="10"/>
       <c r="G19" s="60" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="H19" s="61"/>
       <c r="I19" s="61"/>
@@ -1570,7 +1709,7 @@
       <c r="K19" s="61"/>
       <c r="L19" s="62"/>
       <c r="M19" s="60" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="N19" s="61"/>
       <c r="O19" s="61"/>
@@ -1578,7 +1717,7 @@
       <c r="Q19" s="61"/>
       <c r="R19" s="62"/>
       <c r="S19" s="60" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="T19" s="61"/>
       <c r="U19" s="61"/>
@@ -1586,24 +1725,24 @@
       <c r="W19" s="61"/>
       <c r="X19" s="62"/>
       <c r="Y19" s="10"/>
-      <c r="Z19" s="39"/>
-      <c r="AA19" s="25"/>
-      <c r="AB19" s="25"/>
-      <c r="AC19" s="25"/>
-      <c r="AD19" s="40"/>
+      <c r="Z19" s="38"/>
+      <c r="AA19" s="31"/>
+      <c r="AB19" s="31"/>
+      <c r="AC19" s="31"/>
+      <c r="AD19" s="39"/>
       <c r="AE19">
         <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:31" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="24"/>
-      <c r="B20" s="25"/>
-      <c r="C20" s="25"/>
-      <c r="D20" s="25"/>
-      <c r="E20" s="26"/>
+      <c r="A20" s="30"/>
+      <c r="B20" s="31"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="32"/>
       <c r="F20" s="10"/>
       <c r="G20" s="60" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="H20" s="61"/>
       <c r="I20" s="61"/>
@@ -1611,7 +1750,7 @@
       <c r="K20" s="61"/>
       <c r="L20" s="62"/>
       <c r="M20" s="60" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="N20" s="61"/>
       <c r="O20" s="61"/>
@@ -1619,7 +1758,7 @@
       <c r="Q20" s="61"/>
       <c r="R20" s="62"/>
       <c r="S20" s="60" t="s">
-        <v>6</v>
+        <v>49</v>
       </c>
       <c r="T20" s="61"/>
       <c r="U20" s="61"/>
@@ -1627,24 +1766,24 @@
       <c r="W20" s="61"/>
       <c r="X20" s="62"/>
       <c r="Y20" s="10"/>
-      <c r="Z20" s="39"/>
-      <c r="AA20" s="25"/>
-      <c r="AB20" s="25"/>
-      <c r="AC20" s="25"/>
-      <c r="AD20" s="40"/>
+      <c r="Z20" s="38"/>
+      <c r="AA20" s="31"/>
+      <c r="AB20" s="31"/>
+      <c r="AC20" s="31"/>
+      <c r="AD20" s="39"/>
       <c r="AE20">
         <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:31" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="24"/>
-      <c r="B21" s="25"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="26"/>
+      <c r="A21" s="30"/>
+      <c r="B21" s="31"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="32"/>
       <c r="F21" s="10"/>
       <c r="G21" s="60" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="H21" s="61"/>
       <c r="I21" s="61"/>
@@ -1652,7 +1791,7 @@
       <c r="K21" s="61"/>
       <c r="L21" s="62"/>
       <c r="M21" s="60" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="N21" s="61"/>
       <c r="O21" s="61"/>
@@ -1660,7 +1799,7 @@
       <c r="Q21" s="61"/>
       <c r="R21" s="62"/>
       <c r="S21" s="60" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="T21" s="61"/>
       <c r="U21" s="61"/>
@@ -1668,24 +1807,24 @@
       <c r="W21" s="61"/>
       <c r="X21" s="62"/>
       <c r="Y21" s="10"/>
-      <c r="Z21" s="39"/>
-      <c r="AA21" s="25"/>
-      <c r="AB21" s="25"/>
-      <c r="AC21" s="25"/>
-      <c r="AD21" s="40"/>
+      <c r="Z21" s="38"/>
+      <c r="AA21" s="31"/>
+      <c r="AB21" s="31"/>
+      <c r="AC21" s="31"/>
+      <c r="AD21" s="39"/>
       <c r="AE21">
         <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:31" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="24"/>
-      <c r="B22" s="25"/>
-      <c r="C22" s="25"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="26"/>
+      <c r="A22" s="30"/>
+      <c r="B22" s="31"/>
+      <c r="C22" s="31"/>
+      <c r="D22" s="31"/>
+      <c r="E22" s="32"/>
       <c r="F22" s="10"/>
       <c r="G22" s="60" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="H22" s="61"/>
       <c r="I22" s="61"/>
@@ -1693,7 +1832,7 @@
       <c r="K22" s="61"/>
       <c r="L22" s="62"/>
       <c r="M22" s="60" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="N22" s="61"/>
       <c r="O22" s="61"/>
@@ -1701,7 +1840,7 @@
       <c r="Q22" s="61"/>
       <c r="R22" s="62"/>
       <c r="S22" s="60" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="T22" s="61"/>
       <c r="U22" s="61"/>
@@ -1709,24 +1848,24 @@
       <c r="W22" s="61"/>
       <c r="X22" s="62"/>
       <c r="Y22" s="10"/>
-      <c r="Z22" s="39"/>
-      <c r="AA22" s="25"/>
-      <c r="AB22" s="25"/>
-      <c r="AC22" s="25"/>
-      <c r="AD22" s="40"/>
+      <c r="Z22" s="38"/>
+      <c r="AA22" s="31"/>
+      <c r="AB22" s="31"/>
+      <c r="AC22" s="31"/>
+      <c r="AD22" s="39"/>
       <c r="AE22">
         <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:31" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="24"/>
-      <c r="B23" s="25"/>
-      <c r="C23" s="25"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="26"/>
+      <c r="A23" s="30"/>
+      <c r="B23" s="31"/>
+      <c r="C23" s="31"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="32"/>
       <c r="F23" s="10"/>
       <c r="G23" s="60" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="H23" s="61"/>
       <c r="I23" s="61"/>
@@ -1734,7 +1873,7 @@
       <c r="K23" s="61"/>
       <c r="L23" s="62"/>
       <c r="M23" s="60" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="N23" s="61"/>
       <c r="O23" s="61"/>
@@ -1742,7 +1881,7 @@
       <c r="Q23" s="61"/>
       <c r="R23" s="62"/>
       <c r="S23" s="60" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="T23" s="61"/>
       <c r="U23" s="61"/>
@@ -1750,24 +1889,24 @@
       <c r="W23" s="61"/>
       <c r="X23" s="62"/>
       <c r="Y23" s="10"/>
-      <c r="Z23" s="39"/>
-      <c r="AA23" s="25"/>
-      <c r="AB23" s="25"/>
-      <c r="AC23" s="25"/>
-      <c r="AD23" s="40"/>
+      <c r="Z23" s="38"/>
+      <c r="AA23" s="31"/>
+      <c r="AB23" s="31"/>
+      <c r="AC23" s="31"/>
+      <c r="AD23" s="39"/>
       <c r="AE23">
         <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:31" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="24"/>
-      <c r="B24" s="25"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="26"/>
+      <c r="A24" s="30"/>
+      <c r="B24" s="31"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="32"/>
       <c r="F24" s="10"/>
       <c r="G24" s="60" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H24" s="61"/>
       <c r="I24" s="61"/>
@@ -1775,7 +1914,7 @@
       <c r="K24" s="61"/>
       <c r="L24" s="62"/>
       <c r="M24" s="60" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="N24" s="61"/>
       <c r="O24" s="61"/>
@@ -1783,7 +1922,7 @@
       <c r="Q24" s="61"/>
       <c r="R24" s="62"/>
       <c r="S24" s="60" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="T24" s="61"/>
       <c r="U24" s="61"/>
@@ -1791,21 +1930,21 @@
       <c r="W24" s="61"/>
       <c r="X24" s="62"/>
       <c r="Y24" s="10"/>
-      <c r="Z24" s="39"/>
-      <c r="AA24" s="25"/>
-      <c r="AB24" s="25"/>
-      <c r="AC24" s="25"/>
-      <c r="AD24" s="40"/>
+      <c r="Z24" s="38"/>
+      <c r="AA24" s="31"/>
+      <c r="AB24" s="31"/>
+      <c r="AC24" s="31"/>
+      <c r="AD24" s="39"/>
       <c r="AE24">
         <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:31" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="27"/>
-      <c r="B25" s="28"/>
-      <c r="C25" s="28"/>
-      <c r="D25" s="28"/>
-      <c r="E25" s="29"/>
+      <c r="A25" s="33"/>
+      <c r="B25" s="34"/>
+      <c r="C25" s="34"/>
+      <c r="D25" s="34"/>
+      <c r="E25" s="35"/>
       <c r="F25" s="14"/>
       <c r="G25" s="60" t="s">
         <v>6</v>
@@ -1816,7 +1955,7 @@
       <c r="K25" s="61"/>
       <c r="L25" s="62"/>
       <c r="M25" s="60" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="N25" s="61"/>
       <c r="O25" s="61"/>
@@ -1824,7 +1963,7 @@
       <c r="Q25" s="61"/>
       <c r="R25" s="62"/>
       <c r="S25" s="60" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="T25" s="61"/>
       <c r="U25" s="61"/>
@@ -1832,11 +1971,11 @@
       <c r="W25" s="61"/>
       <c r="X25" s="62"/>
       <c r="Y25" s="14"/>
-      <c r="Z25" s="41"/>
-      <c r="AA25" s="28"/>
-      <c r="AB25" s="28"/>
-      <c r="AC25" s="28"/>
-      <c r="AD25" s="42"/>
+      <c r="Z25" s="40"/>
+      <c r="AA25" s="34"/>
+      <c r="AB25" s="34"/>
+      <c r="AC25" s="34"/>
+      <c r="AD25" s="41"/>
       <c r="AE25">
         <v>21</v>
       </c>
@@ -1848,7 +1987,7 @@
       <c r="D26" s="17"/>
       <c r="E26" s="18"/>
       <c r="F26" s="19"/>
-      <c r="G26" s="36" t="s">
+      <c r="G26" s="57" t="s">
         <v>5</v>
       </c>
       <c r="H26" s="58"/>
@@ -1856,7 +1995,7 @@
       <c r="J26" s="58"/>
       <c r="K26" s="58"/>
       <c r="L26" s="59"/>
-      <c r="M26" s="36" t="s">
+      <c r="M26" s="57" t="s">
         <v>5</v>
       </c>
       <c r="N26" s="58"/>
@@ -1864,7 +2003,7 @@
       <c r="P26" s="58"/>
       <c r="Q26" s="58"/>
       <c r="R26" s="59"/>
-      <c r="S26" s="36" t="s">
+      <c r="S26" s="57" t="s">
         <v>5</v>
       </c>
       <c r="T26" s="58"/>
@@ -1924,26 +2063,26 @@
       <c r="D28" s="5"/>
       <c r="E28" s="8"/>
       <c r="F28" s="10"/>
-      <c r="G28" s="30" t="s">
+      <c r="G28" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="H28" s="31"/>
-      <c r="I28" s="31"/>
-      <c r="J28" s="31"/>
-      <c r="K28" s="31"/>
-      <c r="L28" s="31"/>
-      <c r="M28" s="31"/>
-      <c r="N28" s="31"/>
-      <c r="O28" s="31"/>
-      <c r="P28" s="31"/>
-      <c r="Q28" s="31"/>
-      <c r="R28" s="31"/>
-      <c r="S28" s="31"/>
-      <c r="T28" s="31"/>
-      <c r="U28" s="31"/>
-      <c r="V28" s="31"/>
-      <c r="W28" s="31"/>
-      <c r="X28" s="32"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="22"/>
+      <c r="J28" s="22"/>
+      <c r="K28" s="22"/>
+      <c r="L28" s="22"/>
+      <c r="M28" s="22"/>
+      <c r="N28" s="22"/>
+      <c r="O28" s="22"/>
+      <c r="P28" s="22"/>
+      <c r="Q28" s="22"/>
+      <c r="R28" s="22"/>
+      <c r="S28" s="22"/>
+      <c r="T28" s="22"/>
+      <c r="U28" s="22"/>
+      <c r="V28" s="22"/>
+      <c r="W28" s="22"/>
+      <c r="X28" s="23"/>
       <c r="Y28" s="10"/>
       <c r="Z28" s="5"/>
       <c r="AA28" s="5"/>
@@ -1958,24 +2097,24 @@
       <c r="D29" s="12"/>
       <c r="E29" s="13"/>
       <c r="F29" s="14"/>
-      <c r="G29" s="33"/>
-      <c r="H29" s="34"/>
-      <c r="I29" s="34"/>
-      <c r="J29" s="34"/>
-      <c r="K29" s="34"/>
-      <c r="L29" s="34"/>
-      <c r="M29" s="34"/>
-      <c r="N29" s="34"/>
-      <c r="O29" s="34"/>
-      <c r="P29" s="34"/>
-      <c r="Q29" s="34"/>
-      <c r="R29" s="34"/>
-      <c r="S29" s="34"/>
-      <c r="T29" s="34"/>
-      <c r="U29" s="34"/>
-      <c r="V29" s="34"/>
-      <c r="W29" s="34"/>
-      <c r="X29" s="35"/>
+      <c r="G29" s="24"/>
+      <c r="H29" s="25"/>
+      <c r="I29" s="25"/>
+      <c r="J29" s="25"/>
+      <c r="K29" s="25"/>
+      <c r="L29" s="25"/>
+      <c r="M29" s="25"/>
+      <c r="N29" s="25"/>
+      <c r="O29" s="25"/>
+      <c r="P29" s="25"/>
+      <c r="Q29" s="25"/>
+      <c r="R29" s="25"/>
+      <c r="S29" s="25"/>
+      <c r="T29" s="25"/>
+      <c r="U29" s="25"/>
+      <c r="V29" s="25"/>
+      <c r="W29" s="25"/>
+      <c r="X29" s="26"/>
       <c r="Y29" s="14"/>
       <c r="Z29" s="12"/>
       <c r="AA29" s="12"/>
@@ -2005,42 +2144,25 @@
     </row>
   </sheetData>
   <mergeCells count="56">
-    <mergeCell ref="M25:R25"/>
-    <mergeCell ref="S25:X25"/>
-    <mergeCell ref="M22:R22"/>
-    <mergeCell ref="S22:X22"/>
-    <mergeCell ref="M23:R23"/>
-    <mergeCell ref="S23:X23"/>
-    <mergeCell ref="M24:R24"/>
-    <mergeCell ref="S24:X24"/>
-    <mergeCell ref="M19:R19"/>
-    <mergeCell ref="S19:X19"/>
-    <mergeCell ref="M20:R20"/>
-    <mergeCell ref="S20:X20"/>
-    <mergeCell ref="M21:R21"/>
-    <mergeCell ref="S21:X21"/>
-    <mergeCell ref="M16:R16"/>
-    <mergeCell ref="S16:X16"/>
-    <mergeCell ref="M17:R17"/>
-    <mergeCell ref="S17:X17"/>
-    <mergeCell ref="M18:R18"/>
-    <mergeCell ref="S18:X18"/>
-    <mergeCell ref="M13:R13"/>
-    <mergeCell ref="S13:X13"/>
-    <mergeCell ref="M14:R14"/>
-    <mergeCell ref="S14:X14"/>
-    <mergeCell ref="M15:R15"/>
-    <mergeCell ref="S15:X15"/>
+    <mergeCell ref="G15:L15"/>
+    <mergeCell ref="G28:X29"/>
+    <mergeCell ref="A10:E25"/>
+    <mergeCell ref="Z10:AD25"/>
+    <mergeCell ref="G1:X5"/>
+    <mergeCell ref="G7:X8"/>
+    <mergeCell ref="G26:L26"/>
+    <mergeCell ref="M26:R26"/>
+    <mergeCell ref="S26:X26"/>
+    <mergeCell ref="S10:X10"/>
+    <mergeCell ref="M11:R11"/>
+    <mergeCell ref="S11:X11"/>
+    <mergeCell ref="M12:R12"/>
+    <mergeCell ref="S12:X12"/>
     <mergeCell ref="G22:L22"/>
     <mergeCell ref="G23:L23"/>
     <mergeCell ref="G24:L24"/>
     <mergeCell ref="G25:L25"/>
     <mergeCell ref="M10:R10"/>
-    <mergeCell ref="S10:X10"/>
-    <mergeCell ref="M11:R11"/>
-    <mergeCell ref="S11:X11"/>
-    <mergeCell ref="M12:R12"/>
-    <mergeCell ref="S12:X12"/>
     <mergeCell ref="G16:L16"/>
     <mergeCell ref="G17:L17"/>
     <mergeCell ref="G18:L18"/>
@@ -2052,15 +2174,32 @@
     <mergeCell ref="G12:L12"/>
     <mergeCell ref="G13:L13"/>
     <mergeCell ref="G14:L14"/>
-    <mergeCell ref="G15:L15"/>
-    <mergeCell ref="G28:X29"/>
-    <mergeCell ref="A10:E25"/>
-    <mergeCell ref="Z10:AD25"/>
-    <mergeCell ref="G1:X5"/>
-    <mergeCell ref="G7:X8"/>
-    <mergeCell ref="G26:L26"/>
-    <mergeCell ref="M26:R26"/>
-    <mergeCell ref="S26:X26"/>
+    <mergeCell ref="M13:R13"/>
+    <mergeCell ref="S13:X13"/>
+    <mergeCell ref="M14:R14"/>
+    <mergeCell ref="S14:X14"/>
+    <mergeCell ref="M15:R15"/>
+    <mergeCell ref="S15:X15"/>
+    <mergeCell ref="M16:R16"/>
+    <mergeCell ref="S16:X16"/>
+    <mergeCell ref="M17:R17"/>
+    <mergeCell ref="S17:X17"/>
+    <mergeCell ref="M18:R18"/>
+    <mergeCell ref="S18:X18"/>
+    <mergeCell ref="M19:R19"/>
+    <mergeCell ref="S19:X19"/>
+    <mergeCell ref="M20:R20"/>
+    <mergeCell ref="S20:X20"/>
+    <mergeCell ref="M21:R21"/>
+    <mergeCell ref="S21:X21"/>
+    <mergeCell ref="M25:R25"/>
+    <mergeCell ref="S25:X25"/>
+    <mergeCell ref="M22:R22"/>
+    <mergeCell ref="S22:X22"/>
+    <mergeCell ref="M23:R23"/>
+    <mergeCell ref="S23:X23"/>
+    <mergeCell ref="M24:R24"/>
+    <mergeCell ref="S24:X24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>